<commit_message>
Regeneration of en/fr/es country data books after child program paras updated
</commit_message>
<xml_diff>
--- a/inputs/en/Optima_template.xlsx
+++ b/inputs/en/Optima_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\GitHub\Nutrition\inputs\en\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\modeling\Nutrition\inputs\en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CE69DF-BE4C-4CD2-A66B-1F47C51D0F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412CDB60-4687-4849-96B1-112EA339DEAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15225" yWindow="-18120" windowWidth="29040" windowHeight="17640" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="961" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -2327,8 +2327,8 @@
   </sheetPr>
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3511,7 +3511,7 @@
   </sheetPr>
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -13629,12 +13629,36 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="GEHiGU/wzMESSzNocXwPkaIr4XGdamS9vmVQvyC3AZJHmUXgJGyneI4jc1TC32WmhOi7y0hwZVPwY8duXyz3Tw==" saltValue="r4SSSOoEaaDH7zhAAgw2UA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="45">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B145:B147"/>
+    <mergeCell ref="B148:B150"/>
+    <mergeCell ref="B151:B153"/>
+    <mergeCell ref="B154:B156"/>
+    <mergeCell ref="B128:B130"/>
+    <mergeCell ref="B131:B133"/>
+    <mergeCell ref="B134:B136"/>
+    <mergeCell ref="B137:B139"/>
+    <mergeCell ref="B142:B144"/>
+    <mergeCell ref="B111:B113"/>
+    <mergeCell ref="B114:B116"/>
+    <mergeCell ref="B117:B119"/>
+    <mergeCell ref="B120:B122"/>
+    <mergeCell ref="B125:B127"/>
+    <mergeCell ref="B108:B110"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="B92:B94"/>
+    <mergeCell ref="B95:B97"/>
+    <mergeCell ref="B98:B100"/>
+    <mergeCell ref="B101:B103"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="B67:B69"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -13644,36 +13668,12 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="B108:B110"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="B92:B94"/>
-    <mergeCell ref="B95:B97"/>
-    <mergeCell ref="B98:B100"/>
-    <mergeCell ref="B101:B103"/>
-    <mergeCell ref="B111:B113"/>
-    <mergeCell ref="B114:B116"/>
-    <mergeCell ref="B117:B119"/>
-    <mergeCell ref="B120:B122"/>
-    <mergeCell ref="B125:B127"/>
-    <mergeCell ref="B145:B147"/>
-    <mergeCell ref="B148:B150"/>
-    <mergeCell ref="B151:B153"/>
-    <mergeCell ref="B154:B156"/>
-    <mergeCell ref="B128:B130"/>
-    <mergeCell ref="B131:B133"/>
-    <mergeCell ref="B134:B136"/>
-    <mergeCell ref="B137:B139"/>
-    <mergeCell ref="B142:B144"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -28175,8 +28175,8 @@
   </sheetPr>
   <dimension ref="A1:H163"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -28236,13 +28236,13 @@
         <v>0</v>
       </c>
       <c r="F2" s="85">
-        <v>0.33500000000000002</v>
+        <v>0.39473684210526322</v>
       </c>
       <c r="G2" s="85">
-        <v>0.33500000000000002</v>
+        <v>0.39473684210526322</v>
       </c>
       <c r="H2" s="85">
-        <v>0.33500000000000002</v>
+        <v>0.39473684210526322</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -28256,13 +28256,13 @@
         <v>0</v>
       </c>
       <c r="F3" s="85">
-        <v>0.53134328358208949</v>
+        <v>0.30769230769230765</v>
       </c>
       <c r="G3" s="85">
-        <v>0.53134328358208949</v>
+        <v>0.30769230769230765</v>
       </c>
       <c r="H3" s="85">
-        <v>0.53134328358208949</v>
+        <v>0.30769230769230765</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -28276,13 +28276,13 @@
         <v>0</v>
       </c>
       <c r="F4" s="85">
-        <v>0.38507462686567179</v>
+        <v>0.38507462686567184</v>
       </c>
       <c r="G4" s="85">
-        <v>0.38507462686567179</v>
+        <v>0.38507462686567184</v>
       </c>
       <c r="H4" s="85">
-        <v>0.38507462686567179</v>
+        <v>0.38507462686567184</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -28322,10 +28322,10 @@
         <v>0</v>
       </c>
       <c r="F6" s="85">
-        <v>0.25970149253731339</v>
+        <v>0.25970149253731345</v>
       </c>
       <c r="G6" s="85">
-        <v>0.25970149253731339</v>
+        <v>0.25970149253731345</v>
       </c>
       <c r="H6" s="85">
         <v>0</v>
@@ -28365,10 +28365,10 @@
         <v>0</v>
       </c>
       <c r="F8" s="85">
-        <v>0.25970149253731339</v>
+        <v>0.25970149253731345</v>
       </c>
       <c r="G8" s="85">
-        <v>0.25970149253731339</v>
+        <v>0.25970149253731345</v>
       </c>
       <c r="H8" s="85">
         <v>0</v>
@@ -28411,10 +28411,10 @@
         <v>0</v>
       </c>
       <c r="F10" s="85">
-        <v>0.25970149253731339</v>
+        <v>0.25970149253731345</v>
       </c>
       <c r="G10" s="85">
-        <v>0.25970149253731339</v>
+        <v>0.25970149253731345</v>
       </c>
       <c r="H10" s="85">
         <v>0</v>
@@ -28454,10 +28454,10 @@
         <v>0</v>
       </c>
       <c r="F12" s="85">
-        <v>0.25970149253731339</v>
+        <v>0.25970149253731345</v>
       </c>
       <c r="G12" s="85">
-        <v>0.25970149253731339</v>
+        <v>0.25970149253731345</v>
       </c>
       <c r="H12" s="85">
         <v>0</v>
@@ -28500,10 +28500,10 @@
         <v>0</v>
       </c>
       <c r="F14" s="85">
-        <v>0.25970149253731339</v>
+        <v>0.25970149253731345</v>
       </c>
       <c r="G14" s="85">
-        <v>0.25970149253731339</v>
+        <v>0.25970149253731345</v>
       </c>
       <c r="H14" s="85">
         <v>0</v>
@@ -28543,10 +28543,10 @@
         <v>0</v>
       </c>
       <c r="F16" s="85">
-        <v>0.25970149253731339</v>
+        <v>0.25970149253731345</v>
       </c>
       <c r="G16" s="85">
-        <v>0.25970149253731339</v>
+        <v>0.25970149253731345</v>
       </c>
       <c r="H16" s="85">
         <v>0</v>
@@ -28589,7 +28589,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="85">
-        <v>0.33500000000000002</v>
+        <v>0.7</v>
       </c>
       <c r="G18" s="85">
         <v>0.62</v>
@@ -28632,7 +28632,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="85">
-        <v>0.33500000000000002</v>
+        <v>0.84</v>
       </c>
       <c r="G20" s="85">
         <v>0.62</v>
@@ -28652,13 +28652,13 @@
         <v>338</v>
       </c>
       <c r="D21" s="85">
-        <v>0.7</v>
+        <v>0.28260869565217389</v>
       </c>
       <c r="E21" s="85">
         <v>0</v>
       </c>
       <c r="F21" s="85">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G21" s="85">
         <v>0</v>
@@ -28678,7 +28678,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="85">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G22" s="85">
         <v>0</v>
@@ -28698,13 +28698,13 @@
         <v>338</v>
       </c>
       <c r="D23" s="85">
-        <v>0.7</v>
+        <v>0.28260869565217389</v>
       </c>
       <c r="E23" s="85">
         <v>0</v>
       </c>
       <c r="F23" s="85">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G23" s="85">
         <v>0</v>
@@ -28724,7 +28724,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="85">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G24" s="85">
         <v>0</v>
@@ -28744,13 +28744,13 @@
         <v>338</v>
       </c>
       <c r="D25" s="85">
-        <v>0.7</v>
+        <v>0.28260869565217389</v>
       </c>
       <c r="E25" s="85">
         <v>0</v>
       </c>
       <c r="F25" s="85">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G25" s="85">
         <v>0</v>
@@ -28770,7 +28770,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="85">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G26" s="85">
         <v>0</v>
@@ -28796,7 +28796,7 @@
         <v>1</v>
       </c>
       <c r="F27" s="85">
-        <v>0.33500000000000002</v>
+        <v>1</v>
       </c>
       <c r="G27" s="85">
         <v>1</v>
@@ -28816,7 +28816,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="85">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G28" s="85">
         <v>0</v>
@@ -28836,7 +28836,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="85">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G29" s="85">
         <v>0</v>
@@ -28862,7 +28862,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="85">
-        <v>0.33500000000000002</v>
+        <v>1</v>
       </c>
       <c r="G30" s="85">
         <v>1</v>
@@ -28882,7 +28882,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="85">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G31" s="85">
         <v>0</v>
@@ -28902,7 +28902,7 @@
         <v>0</v>
       </c>
       <c r="F32" s="85">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G32" s="85">
         <v>0</v>
@@ -28928,7 +28928,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="85">
-        <v>0.33500000000000002</v>
+        <v>1</v>
       </c>
       <c r="G33" s="85">
         <v>1</v>
@@ -28948,7 +28948,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="85">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G34" s="85">
         <v>0</v>
@@ -28968,7 +28968,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="85">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G35" s="85">
         <v>0</v>
@@ -28994,7 +28994,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="85">
-        <v>0.33500000000000002</v>
+        <v>1</v>
       </c>
       <c r="G36" s="85">
         <v>1</v>
@@ -29014,7 +29014,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="85">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G37" s="85">
         <v>0</v>
@@ -29034,7 +29034,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="85">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G38" s="85">
         <v>0</v>
@@ -29060,7 +29060,7 @@
         <v>1</v>
       </c>
       <c r="F39" s="85">
-        <v>0.33500000000000002</v>
+        <v>1</v>
       </c>
       <c r="G39" s="85">
         <v>1</v>
@@ -29080,7 +29080,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="85">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G40" s="85">
         <v>0</v>
@@ -29100,7 +29100,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="85">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G41" s="85">
         <v>0</v>
@@ -29126,7 +29126,7 @@
         <v>0.3</v>
       </c>
       <c r="F42" s="85">
-        <v>0.33500000000000002</v>
+        <v>0.3</v>
       </c>
       <c r="G42" s="85">
         <v>0.3</v>
@@ -29146,7 +29146,7 @@
         <v>0.5</v>
       </c>
       <c r="F43" s="85">
-        <v>0.33500000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="G43" s="85">
         <v>0.5</v>
@@ -29166,7 +29166,7 @@
         <v>0.65</v>
       </c>
       <c r="F44" s="85">
-        <v>0.33500000000000002</v>
+        <v>0.65</v>
       </c>
       <c r="G44" s="85">
         <v>0.65</v>
@@ -29189,7 +29189,7 @@
         <v>0.3</v>
       </c>
       <c r="F45" s="85">
-        <v>0.33500000000000002</v>
+        <v>0.3</v>
       </c>
       <c r="G45" s="85">
         <v>0.3</v>
@@ -29209,7 +29209,7 @@
         <v>0.49</v>
       </c>
       <c r="F46" s="85">
-        <v>0.33500000000000002</v>
+        <v>0.49</v>
       </c>
       <c r="G46" s="85">
         <v>0.49</v>
@@ -29229,7 +29229,7 @@
         <v>0.52</v>
       </c>
       <c r="F47" s="85">
-        <v>0.33500000000000002</v>
+        <v>0.52</v>
       </c>
       <c r="G47" s="85">
         <v>0.52</v>
@@ -29255,7 +29255,7 @@
         <v>0.88</v>
       </c>
       <c r="F48" s="85">
-        <v>0.33500000000000002</v>
+        <v>0.88</v>
       </c>
       <c r="G48" s="85">
         <v>0.88</v>
@@ -29269,19 +29269,19 @@
         <v>339</v>
       </c>
       <c r="D49" s="85">
-        <v>0.93</v>
+        <v>0.78409090909090906</v>
       </c>
       <c r="E49" s="85">
-        <v>0.93</v>
+        <v>0.78409090909090906</v>
       </c>
       <c r="F49" s="85">
-        <v>0.33500000000000002</v>
+        <v>0.78409090909090906</v>
       </c>
       <c r="G49" s="85">
-        <v>0.93</v>
+        <v>0.78409090909090906</v>
       </c>
       <c r="H49" s="85">
-        <v>0.93</v>
+        <v>0.78409090909090906</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -29295,19 +29295,19 @@
         <v>338</v>
       </c>
       <c r="D50" s="85">
-        <v>1</v>
+        <v>0.88372093023255816</v>
       </c>
       <c r="E50" s="85">
-        <v>1</v>
+        <v>0.88372093023255816</v>
       </c>
       <c r="F50" s="85">
-        <v>0.33500000000000002</v>
+        <v>0.88372093023255816</v>
       </c>
       <c r="G50" s="85">
-        <v>1</v>
+        <v>0.88372093023255816</v>
       </c>
       <c r="H50" s="85">
-        <v>1</v>
+        <v>0.88372093023255816</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -29321,7 +29321,7 @@
         <v>0.86</v>
       </c>
       <c r="F51" s="85">
-        <v>0.33500000000000002</v>
+        <v>0.86</v>
       </c>
       <c r="G51" s="85">
         <v>0.86</v>
@@ -29347,7 +29347,7 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="F52" s="85">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G52" s="85">
         <v>0</v>
@@ -29367,7 +29367,7 @@
         <v>0.51</v>
       </c>
       <c r="F53" s="85">
-        <v>0.33500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G53" s="85">
         <v>0</v>
@@ -29429,15 +29429,15 @@
       </c>
       <c r="F57" s="85">
         <f t="shared" si="0"/>
-        <v>0.30150000000000005</v>
+        <v>0.35526315789473689</v>
       </c>
       <c r="G57" s="85">
         <f t="shared" si="0"/>
-        <v>0.30150000000000005</v>
+        <v>0.35526315789473689</v>
       </c>
       <c r="H57" s="85">
         <f t="shared" si="0"/>
-        <v>0.30150000000000005</v>
+        <v>0.35526315789473689</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -29454,15 +29454,15 @@
       </c>
       <c r="F58" s="85">
         <f t="shared" si="0"/>
-        <v>0.47820895522388057</v>
+        <v>0.27692307692307688</v>
       </c>
       <c r="G58" s="85">
         <f t="shared" si="0"/>
-        <v>0.47820895522388057</v>
+        <v>0.27692307692307688</v>
       </c>
       <c r="H58" s="85">
         <f t="shared" si="0"/>
-        <v>0.47820895522388057</v>
+        <v>0.27692307692307688</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -29479,15 +29479,15 @@
       </c>
       <c r="F59" s="85">
         <f t="shared" si="0"/>
-        <v>0.3465671641791046</v>
+        <v>0.34656716417910466</v>
       </c>
       <c r="G59" s="85">
         <f t="shared" si="0"/>
-        <v>0.3465671641791046</v>
+        <v>0.34656716417910466</v>
       </c>
       <c r="H59" s="85">
         <f t="shared" si="0"/>
-        <v>0.3465671641791046</v>
+        <v>0.34656716417910466</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -29535,11 +29535,11 @@
       </c>
       <c r="F61" s="85">
         <f t="shared" si="0"/>
-        <v>0.23373134328358205</v>
+        <v>0.23373134328358211</v>
       </c>
       <c r="G61" s="85">
         <f t="shared" si="0"/>
-        <v>0.23373134328358205</v>
+        <v>0.23373134328358211</v>
       </c>
       <c r="H61" s="85">
         <f t="shared" si="0"/>
@@ -29588,11 +29588,11 @@
       </c>
       <c r="F63" s="85">
         <f t="shared" si="0"/>
-        <v>0.23373134328358205</v>
+        <v>0.23373134328358211</v>
       </c>
       <c r="G63" s="85">
         <f t="shared" si="0"/>
-        <v>0.23373134328358205</v>
+        <v>0.23373134328358211</v>
       </c>
       <c r="H63" s="85">
         <f t="shared" si="0"/>
@@ -29644,11 +29644,11 @@
       </c>
       <c r="F65" s="85">
         <f t="shared" si="0"/>
-        <v>0.23373134328358205</v>
+        <v>0.23373134328358211</v>
       </c>
       <c r="G65" s="85">
         <f t="shared" si="0"/>
-        <v>0.23373134328358205</v>
+        <v>0.23373134328358211</v>
       </c>
       <c r="H65" s="85">
         <f t="shared" si="0"/>
@@ -29697,11 +29697,11 @@
       </c>
       <c r="F67" s="85">
         <f t="shared" si="1"/>
-        <v>0.23373134328358205</v>
+        <v>0.23373134328358211</v>
       </c>
       <c r="G67" s="85">
         <f t="shared" si="1"/>
-        <v>0.23373134328358205</v>
+        <v>0.23373134328358211</v>
       </c>
       <c r="H67" s="85">
         <f t="shared" si="1"/>
@@ -29753,11 +29753,11 @@
       </c>
       <c r="F69" s="85">
         <f t="shared" si="1"/>
-        <v>0.23373134328358205</v>
+        <v>0.23373134328358211</v>
       </c>
       <c r="G69" s="85">
         <f t="shared" si="1"/>
-        <v>0.23373134328358205</v>
+        <v>0.23373134328358211</v>
       </c>
       <c r="H69" s="85">
         <f t="shared" si="1"/>
@@ -29806,11 +29806,11 @@
       </c>
       <c r="F71" s="85">
         <f t="shared" si="1"/>
-        <v>0.23373134328358205</v>
+        <v>0.23373134328358211</v>
       </c>
       <c r="G71" s="85">
         <f t="shared" si="1"/>
-        <v>0.23373134328358205</v>
+        <v>0.23373134328358211</v>
       </c>
       <c r="H71" s="85">
         <f t="shared" si="1"/>
@@ -29862,7 +29862,7 @@
       </c>
       <c r="F73" s="85">
         <f t="shared" si="1"/>
-        <v>0.30150000000000005</v>
+        <v>0.63</v>
       </c>
       <c r="G73" s="85">
         <f t="shared" si="1"/>
@@ -29915,7 +29915,7 @@
       </c>
       <c r="F75" s="85">
         <f t="shared" si="1"/>
-        <v>0.30150000000000005</v>
+        <v>0.75600000000000001</v>
       </c>
       <c r="G75" s="85">
         <f t="shared" si="1"/>
@@ -29938,7 +29938,7 @@
       </c>
       <c r="D76" s="85">
         <f t="shared" si="1"/>
-        <v>0.63</v>
+        <v>0.2543478260869565</v>
       </c>
       <c r="E76" s="85">
         <f t="shared" si="1"/>
@@ -29946,7 +29946,7 @@
       </c>
       <c r="F76" s="85">
         <f t="shared" si="1"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G76" s="85">
         <f t="shared" si="1"/>
@@ -29971,7 +29971,7 @@
       </c>
       <c r="F77" s="85">
         <f t="shared" si="2"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G77" s="85">
         <f t="shared" si="2"/>
@@ -29994,7 +29994,7 @@
       </c>
       <c r="D78" s="85">
         <f t="shared" si="2"/>
-        <v>0.63</v>
+        <v>0.2543478260869565</v>
       </c>
       <c r="E78" s="85">
         <f t="shared" si="2"/>
@@ -30002,7 +30002,7 @@
       </c>
       <c r="F78" s="85">
         <f t="shared" si="2"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G78" s="85">
         <f t="shared" si="2"/>
@@ -30027,7 +30027,7 @@
       </c>
       <c r="F79" s="85">
         <f t="shared" si="2"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G79" s="85">
         <f t="shared" si="2"/>
@@ -30050,7 +30050,7 @@
       </c>
       <c r="D80" s="85">
         <f t="shared" si="2"/>
-        <v>0.63</v>
+        <v>0.2543478260869565</v>
       </c>
       <c r="E80" s="85">
         <f t="shared" si="2"/>
@@ -30058,7 +30058,7 @@
       </c>
       <c r="F80" s="85">
         <f t="shared" si="2"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G80" s="85">
         <f t="shared" si="2"/>
@@ -30083,7 +30083,7 @@
       </c>
       <c r="F81" s="85">
         <f t="shared" si="2"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G81" s="85">
         <f t="shared" si="2"/>
@@ -30114,7 +30114,7 @@
       </c>
       <c r="F82" s="85">
         <f t="shared" si="2"/>
-        <v>0.30150000000000005</v>
+        <v>0.9</v>
       </c>
       <c r="G82" s="85">
         <f t="shared" si="2"/>
@@ -30139,7 +30139,7 @@
       </c>
       <c r="F83" s="85">
         <f t="shared" si="2"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G83" s="85">
         <f t="shared" si="2"/>
@@ -30164,7 +30164,7 @@
       </c>
       <c r="F84" s="85">
         <f t="shared" si="2"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G84" s="85">
         <f t="shared" si="2"/>
@@ -30195,7 +30195,7 @@
       </c>
       <c r="F85" s="85">
         <f t="shared" si="2"/>
-        <v>0.30150000000000005</v>
+        <v>0.9</v>
       </c>
       <c r="G85" s="85">
         <f t="shared" si="2"/>
@@ -30220,7 +30220,7 @@
       </c>
       <c r="F86" s="85">
         <f t="shared" si="2"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G86" s="85">
         <f t="shared" si="2"/>
@@ -30245,7 +30245,7 @@
       </c>
       <c r="F87" s="85">
         <f t="shared" si="3"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G87" s="85">
         <f t="shared" si="3"/>
@@ -30276,7 +30276,7 @@
       </c>
       <c r="F88" s="85">
         <f t="shared" si="3"/>
-        <v>0.30150000000000005</v>
+        <v>0.9</v>
       </c>
       <c r="G88" s="85">
         <f t="shared" si="3"/>
@@ -30301,7 +30301,7 @@
       </c>
       <c r="F89" s="85">
         <f t="shared" si="3"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G89" s="85">
         <f t="shared" si="3"/>
@@ -30326,7 +30326,7 @@
       </c>
       <c r="F90" s="85">
         <f t="shared" si="3"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G90" s="85">
         <f t="shared" si="3"/>
@@ -30357,7 +30357,7 @@
       </c>
       <c r="F91" s="85">
         <f t="shared" si="3"/>
-        <v>0.30150000000000005</v>
+        <v>0.9</v>
       </c>
       <c r="G91" s="85">
         <f t="shared" si="3"/>
@@ -30382,7 +30382,7 @@
       </c>
       <c r="F92" s="85">
         <f t="shared" si="3"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G92" s="85">
         <f t="shared" si="3"/>
@@ -30407,7 +30407,7 @@
       </c>
       <c r="F93" s="85">
         <f t="shared" si="3"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G93" s="85">
         <f t="shared" si="3"/>
@@ -30438,7 +30438,7 @@
       </c>
       <c r="F94" s="85">
         <f t="shared" si="3"/>
-        <v>0.30150000000000005</v>
+        <v>0.9</v>
       </c>
       <c r="G94" s="85">
         <f t="shared" si="3"/>
@@ -30463,7 +30463,7 @@
       </c>
       <c r="F95" s="85">
         <f t="shared" si="3"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G95" s="85">
         <f t="shared" si="3"/>
@@ -30488,7 +30488,7 @@
       </c>
       <c r="F96" s="85">
         <f t="shared" si="3"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G96" s="85">
         <f t="shared" si="3"/>
@@ -30519,7 +30519,7 @@
       </c>
       <c r="F97" s="85">
         <f t="shared" si="4"/>
-        <v>0.30150000000000005</v>
+        <v>0.27</v>
       </c>
       <c r="G97" s="85">
         <f t="shared" si="4"/>
@@ -30544,7 +30544,7 @@
       </c>
       <c r="F98" s="85">
         <f t="shared" si="4"/>
-        <v>0.30150000000000005</v>
+        <v>0.45</v>
       </c>
       <c r="G98" s="85">
         <f t="shared" si="4"/>
@@ -30569,7 +30569,7 @@
       </c>
       <c r="F99" s="85">
         <f t="shared" si="4"/>
-        <v>0.30150000000000005</v>
+        <v>0.58500000000000008</v>
       </c>
       <c r="G99" s="85">
         <f t="shared" si="4"/>
@@ -30597,7 +30597,7 @@
       </c>
       <c r="F100" s="85">
         <f t="shared" si="4"/>
-        <v>0.30150000000000005</v>
+        <v>0.27</v>
       </c>
       <c r="G100" s="85">
         <f t="shared" si="4"/>
@@ -30622,7 +30622,7 @@
       </c>
       <c r="F101" s="85">
         <f t="shared" si="4"/>
-        <v>0.30150000000000005</v>
+        <v>0.441</v>
       </c>
       <c r="G101" s="85">
         <f t="shared" si="4"/>
@@ -30647,7 +30647,7 @@
       </c>
       <c r="F102" s="85">
         <f t="shared" si="4"/>
-        <v>0.30150000000000005</v>
+        <v>0.46800000000000003</v>
       </c>
       <c r="G102" s="85">
         <f t="shared" si="4"/>
@@ -30678,7 +30678,7 @@
       </c>
       <c r="F103" s="85">
         <f t="shared" si="4"/>
-        <v>0.30150000000000005</v>
+        <v>0.79200000000000004</v>
       </c>
       <c r="G103" s="85">
         <f t="shared" si="4"/>
@@ -30695,23 +30695,23 @@
       </c>
       <c r="D104" s="85">
         <f t="shared" si="4"/>
-        <v>0.83700000000000008</v>
+        <v>0.70568181818181819</v>
       </c>
       <c r="E104" s="85">
         <f t="shared" si="4"/>
-        <v>0.83700000000000008</v>
+        <v>0.70568181818181819</v>
       </c>
       <c r="F104" s="85">
         <f t="shared" si="4"/>
-        <v>0.30150000000000005</v>
+        <v>0.70568181818181819</v>
       </c>
       <c r="G104" s="85">
         <f t="shared" si="4"/>
-        <v>0.83700000000000008</v>
+        <v>0.70568181818181819</v>
       </c>
       <c r="H104" s="85">
         <f t="shared" si="4"/>
-        <v>0.83700000000000008</v>
+        <v>0.70568181818181819</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -30726,23 +30726,23 @@
       </c>
       <c r="D105" s="85">
         <f t="shared" si="4"/>
-        <v>0.9</v>
+        <v>0.79534883720930238</v>
       </c>
       <c r="E105" s="85">
         <f t="shared" si="4"/>
-        <v>0.9</v>
+        <v>0.79534883720930238</v>
       </c>
       <c r="F105" s="85">
         <f t="shared" si="4"/>
-        <v>0.30150000000000005</v>
+        <v>0.79534883720930238</v>
       </c>
       <c r="G105" s="85">
         <f t="shared" si="4"/>
-        <v>0.9</v>
+        <v>0.79534883720930238</v>
       </c>
       <c r="H105" s="85">
         <f t="shared" si="4"/>
-        <v>0.9</v>
+        <v>0.79534883720930238</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -30759,7 +30759,7 @@
       </c>
       <c r="F106" s="85">
         <f t="shared" si="4"/>
-        <v>0.30150000000000005</v>
+        <v>0.77400000000000002</v>
       </c>
       <c r="G106" s="85">
         <f t="shared" si="4"/>
@@ -30790,7 +30790,7 @@
       </c>
       <c r="F107" s="85">
         <f t="shared" si="5"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G107" s="85">
         <f t="shared" si="5"/>
@@ -30815,7 +30815,7 @@
       </c>
       <c r="F108" s="85">
         <f t="shared" si="5"/>
-        <v>0.30150000000000005</v>
+        <v>0</v>
       </c>
       <c r="G108" s="85">
         <f t="shared" si="5"/>
@@ -30879,15 +30879,15 @@
       </c>
       <c r="F112" s="85">
         <f t="shared" si="6"/>
-        <v>0.35175000000000006</v>
+        <v>0.41447368421052638</v>
       </c>
       <c r="G112" s="85">
         <f t="shared" si="6"/>
-        <v>0.35175000000000006</v>
+        <v>0.41447368421052638</v>
       </c>
       <c r="H112" s="85">
         <f t="shared" si="6"/>
-        <v>0.35175000000000006</v>
+        <v>0.41447368421052638</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -30904,15 +30904,15 @@
       </c>
       <c r="F113" s="85">
         <f t="shared" si="6"/>
-        <v>0.55791044776119403</v>
+        <v>0.32307692307692304</v>
       </c>
       <c r="G113" s="85">
         <f t="shared" si="6"/>
-        <v>0.55791044776119403</v>
+        <v>0.32307692307692304</v>
       </c>
       <c r="H113" s="85">
         <f t="shared" si="6"/>
-        <v>0.55791044776119403</v>
+        <v>0.32307692307692304</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -30929,15 +30929,15 @@
       </c>
       <c r="F114" s="85">
         <f t="shared" si="6"/>
-        <v>0.40432835820895541</v>
+        <v>0.40432835820895546</v>
       </c>
       <c r="G114" s="85">
         <f t="shared" si="6"/>
-        <v>0.40432835820895541</v>
+        <v>0.40432835820895546</v>
       </c>
       <c r="H114" s="85">
         <f t="shared" si="6"/>
-        <v>0.40432835820895541</v>
+        <v>0.40432835820895546</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -30985,11 +30985,11 @@
       </c>
       <c r="F116" s="85">
         <f t="shared" si="6"/>
-        <v>0.27268656716417905</v>
+        <v>0.27268656716417916</v>
       </c>
       <c r="G116" s="85">
         <f t="shared" si="6"/>
-        <v>0.27268656716417905</v>
+        <v>0.27268656716417916</v>
       </c>
       <c r="H116" s="85">
         <f t="shared" si="6"/>
@@ -31038,11 +31038,11 @@
       </c>
       <c r="F118" s="85">
         <f t="shared" si="6"/>
-        <v>0.27268656716417905</v>
+        <v>0.27268656716417916</v>
       </c>
       <c r="G118" s="85">
         <f t="shared" si="6"/>
-        <v>0.27268656716417905</v>
+        <v>0.27268656716417916</v>
       </c>
       <c r="H118" s="85">
         <f t="shared" si="6"/>
@@ -31094,11 +31094,11 @@
       </c>
       <c r="F120" s="85">
         <f t="shared" si="6"/>
-        <v>0.27268656716417905</v>
+        <v>0.27268656716417916</v>
       </c>
       <c r="G120" s="85">
         <f t="shared" si="6"/>
-        <v>0.27268656716417905</v>
+        <v>0.27268656716417916</v>
       </c>
       <c r="H120" s="85">
         <f t="shared" si="6"/>
@@ -31147,11 +31147,11 @@
       </c>
       <c r="F122" s="85">
         <f t="shared" si="7"/>
-        <v>0.27268656716417905</v>
+        <v>0.27268656716417916</v>
       </c>
       <c r="G122" s="85">
         <f t="shared" si="7"/>
-        <v>0.27268656716417905</v>
+        <v>0.27268656716417916</v>
       </c>
       <c r="H122" s="85">
         <f t="shared" si="7"/>
@@ -31203,11 +31203,11 @@
       </c>
       <c r="F124" s="85">
         <f t="shared" si="7"/>
-        <v>0.27268656716417905</v>
+        <v>0.27268656716417916</v>
       </c>
       <c r="G124" s="85">
         <f t="shared" si="7"/>
-        <v>0.27268656716417905</v>
+        <v>0.27268656716417916</v>
       </c>
       <c r="H124" s="85">
         <f t="shared" si="7"/>
@@ -31256,11 +31256,11 @@
       </c>
       <c r="F126" s="85">
         <f t="shared" si="7"/>
-        <v>0.27268656716417905</v>
+        <v>0.27268656716417916</v>
       </c>
       <c r="G126" s="85">
         <f t="shared" si="7"/>
-        <v>0.27268656716417905</v>
+        <v>0.27268656716417916</v>
       </c>
       <c r="H126" s="85">
         <f t="shared" si="7"/>
@@ -31312,7 +31312,7 @@
       </c>
       <c r="F128" s="85">
         <f t="shared" si="7"/>
-        <v>0.35175000000000006</v>
+        <v>0.73499999999999999</v>
       </c>
       <c r="G128" s="85">
         <f t="shared" si="7"/>
@@ -31365,7 +31365,7 @@
       </c>
       <c r="F130" s="85">
         <f t="shared" si="7"/>
-        <v>0.35175000000000006</v>
+        <v>0.88200000000000001</v>
       </c>
       <c r="G130" s="85">
         <f t="shared" si="7"/>
@@ -31388,7 +31388,7 @@
       </c>
       <c r="D131" s="85">
         <f t="shared" si="7"/>
-        <v>0.73499999999999999</v>
+        <v>0.29673913043478262</v>
       </c>
       <c r="E131" s="85">
         <f t="shared" si="7"/>
@@ -31396,7 +31396,7 @@
       </c>
       <c r="F131" s="85">
         <f t="shared" si="7"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G131" s="85">
         <f t="shared" si="7"/>
@@ -31421,7 +31421,7 @@
       </c>
       <c r="F132" s="85">
         <f t="shared" si="8"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G132" s="85">
         <f t="shared" si="8"/>
@@ -31444,7 +31444,7 @@
       </c>
       <c r="D133" s="85">
         <f t="shared" si="8"/>
-        <v>0.73499999999999999</v>
+        <v>0.29673913043478262</v>
       </c>
       <c r="E133" s="85">
         <f t="shared" si="8"/>
@@ -31452,7 +31452,7 @@
       </c>
       <c r="F133" s="85">
         <f t="shared" si="8"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G133" s="85">
         <f t="shared" si="8"/>
@@ -31477,7 +31477,7 @@
       </c>
       <c r="F134" s="85">
         <f t="shared" si="8"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G134" s="85">
         <f t="shared" si="8"/>
@@ -31500,7 +31500,7 @@
       </c>
       <c r="D135" s="85">
         <f t="shared" si="8"/>
-        <v>0.73499999999999999</v>
+        <v>0.29673913043478262</v>
       </c>
       <c r="E135" s="85">
         <f t="shared" si="8"/>
@@ -31508,7 +31508,7 @@
       </c>
       <c r="F135" s="85">
         <f t="shared" si="8"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G135" s="85">
         <f t="shared" si="8"/>
@@ -31533,7 +31533,7 @@
       </c>
       <c r="F136" s="85">
         <f t="shared" si="8"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G136" s="85">
         <f t="shared" si="8"/>
@@ -31564,7 +31564,7 @@
       </c>
       <c r="F137" s="85">
         <f t="shared" si="8"/>
-        <v>0.35175000000000006</v>
+        <v>1.05</v>
       </c>
       <c r="G137" s="85">
         <f t="shared" si="8"/>
@@ -31589,7 +31589,7 @@
       </c>
       <c r="F138" s="85">
         <f t="shared" si="8"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G138" s="85">
         <f t="shared" si="8"/>
@@ -31614,7 +31614,7 @@
       </c>
       <c r="F139" s="85">
         <f t="shared" si="8"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G139" s="85">
         <f t="shared" si="8"/>
@@ -31645,7 +31645,7 @@
       </c>
       <c r="F140" s="85">
         <f t="shared" si="8"/>
-        <v>0.35175000000000006</v>
+        <v>1.05</v>
       </c>
       <c r="G140" s="85">
         <f t="shared" si="8"/>
@@ -31670,7 +31670,7 @@
       </c>
       <c r="F141" s="85">
         <f t="shared" si="8"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G141" s="85">
         <f t="shared" si="8"/>
@@ -31695,7 +31695,7 @@
       </c>
       <c r="F142" s="85">
         <f t="shared" si="9"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G142" s="85">
         <f t="shared" si="9"/>
@@ -31726,7 +31726,7 @@
       </c>
       <c r="F143" s="85">
         <f t="shared" si="9"/>
-        <v>0.35175000000000006</v>
+        <v>1.05</v>
       </c>
       <c r="G143" s="85">
         <f t="shared" si="9"/>
@@ -31751,7 +31751,7 @@
       </c>
       <c r="F144" s="85">
         <f t="shared" si="9"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G144" s="85">
         <f t="shared" si="9"/>
@@ -31776,7 +31776,7 @@
       </c>
       <c r="F145" s="85">
         <f t="shared" si="9"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G145" s="85">
         <f t="shared" si="9"/>
@@ -31807,7 +31807,7 @@
       </c>
       <c r="F146" s="85">
         <f t="shared" si="9"/>
-        <v>0.35175000000000006</v>
+        <v>1.05</v>
       </c>
       <c r="G146" s="85">
         <f t="shared" si="9"/>
@@ -31832,7 +31832,7 @@
       </c>
       <c r="F147" s="85">
         <f t="shared" si="9"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G147" s="85">
         <f t="shared" si="9"/>
@@ -31857,7 +31857,7 @@
       </c>
       <c r="F148" s="85">
         <f t="shared" si="9"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G148" s="85">
         <f t="shared" si="9"/>
@@ -31888,7 +31888,7 @@
       </c>
       <c r="F149" s="85">
         <f t="shared" si="9"/>
-        <v>0.35175000000000006</v>
+        <v>1.05</v>
       </c>
       <c r="G149" s="85">
         <f t="shared" si="9"/>
@@ -31913,7 +31913,7 @@
       </c>
       <c r="F150" s="85">
         <f t="shared" si="9"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G150" s="85">
         <f t="shared" si="9"/>
@@ -31938,7 +31938,7 @@
       </c>
       <c r="F151" s="85">
         <f t="shared" si="9"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G151" s="85">
         <f t="shared" si="9"/>
@@ -31969,7 +31969,7 @@
       </c>
       <c r="F152" s="85">
         <f t="shared" si="10"/>
-        <v>0.35175000000000006</v>
+        <v>0.315</v>
       </c>
       <c r="G152" s="85">
         <f t="shared" si="10"/>
@@ -31994,7 +31994,7 @@
       </c>
       <c r="F153" s="85">
         <f t="shared" si="10"/>
-        <v>0.35175000000000006</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="G153" s="85">
         <f t="shared" si="10"/>
@@ -32019,7 +32019,7 @@
       </c>
       <c r="F154" s="85">
         <f t="shared" si="10"/>
-        <v>0.35175000000000006</v>
+        <v>0.68250000000000011</v>
       </c>
       <c r="G154" s="85">
         <f t="shared" si="10"/>
@@ -32047,7 +32047,7 @@
       </c>
       <c r="F155" s="85">
         <f t="shared" si="10"/>
-        <v>0.35175000000000006</v>
+        <v>0.315</v>
       </c>
       <c r="G155" s="85">
         <f t="shared" si="10"/>
@@ -32072,7 +32072,7 @@
       </c>
       <c r="F156" s="85">
         <f t="shared" si="10"/>
-        <v>0.35175000000000006</v>
+        <v>0.51449999999999996</v>
       </c>
       <c r="G156" s="85">
         <f t="shared" si="10"/>
@@ -32097,7 +32097,7 @@
       </c>
       <c r="F157" s="85">
         <f t="shared" si="10"/>
-        <v>0.35175000000000006</v>
+        <v>0.54600000000000004</v>
       </c>
       <c r="G157" s="85">
         <f t="shared" si="10"/>
@@ -32128,7 +32128,7 @@
       </c>
       <c r="F158" s="85">
         <f t="shared" si="10"/>
-        <v>0.35175000000000006</v>
+        <v>0.92400000000000004</v>
       </c>
       <c r="G158" s="85">
         <f t="shared" si="10"/>
@@ -32145,23 +32145,23 @@
       </c>
       <c r="D159" s="85">
         <f t="shared" si="10"/>
-        <v>0.97650000000000015</v>
+        <v>0.8232954545454545</v>
       </c>
       <c r="E159" s="85">
         <f t="shared" si="10"/>
-        <v>0.97650000000000015</v>
+        <v>0.8232954545454545</v>
       </c>
       <c r="F159" s="85">
         <f t="shared" si="10"/>
-        <v>0.35175000000000006</v>
+        <v>0.8232954545454545</v>
       </c>
       <c r="G159" s="85">
         <f t="shared" si="10"/>
-        <v>0.97650000000000015</v>
+        <v>0.8232954545454545</v>
       </c>
       <c r="H159" s="85">
         <f t="shared" si="10"/>
-        <v>0.97650000000000015</v>
+        <v>0.8232954545454545</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
@@ -32176,23 +32176,23 @@
       </c>
       <c r="D160" s="85">
         <f t="shared" si="10"/>
-        <v>1.05</v>
+        <v>0.9279069767441861</v>
       </c>
       <c r="E160" s="85">
         <f t="shared" si="10"/>
-        <v>1.05</v>
+        <v>0.9279069767441861</v>
       </c>
       <c r="F160" s="85">
         <f t="shared" si="10"/>
-        <v>0.35175000000000006</v>
+        <v>0.9279069767441861</v>
       </c>
       <c r="G160" s="85">
         <f t="shared" si="10"/>
-        <v>1.05</v>
+        <v>0.9279069767441861</v>
       </c>
       <c r="H160" s="85">
         <f t="shared" si="10"/>
-        <v>1.05</v>
+        <v>0.9279069767441861</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
@@ -32209,7 +32209,7 @@
       </c>
       <c r="F161" s="85">
         <f t="shared" si="10"/>
-        <v>0.35175000000000006</v>
+        <v>0.90300000000000002</v>
       </c>
       <c r="G161" s="85">
         <f t="shared" si="10"/>
@@ -32240,7 +32240,7 @@
       </c>
       <c r="F162" s="85">
         <f t="shared" si="11"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G162" s="85">
         <f t="shared" si="11"/>
@@ -32265,7 +32265,7 @@
       </c>
       <c r="F163" s="85">
         <f t="shared" si="11"/>
-        <v>0.35175000000000006</v>
+        <v>0</v>
       </c>
       <c r="G163" s="85">
         <f t="shared" si="11"/>

</xml_diff>

<commit_message>
updated the top level books with new font size
</commit_message>
<xml_diff>
--- a/inputs/en/Optima_template.xlsx
+++ b/inputs/en/Optima_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\modeling\Nutrition\inputs\en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412CDB60-4687-4849-96B1-112EA339DEAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D5860E-EC3F-4805-ABA2-2CA7064D52EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="961" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="961" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -1446,7 +1446,7 @@
     <numFmt numFmtId="167" formatCode="0.0%"/>
     <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1562,6 +1562,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1707,7 +1713,7 @@
     <xf numFmtId="9" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1958,6 +1964,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Comma 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
@@ -3511,7 +3520,7 @@
   </sheetPr>
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -13629,6 +13638,42 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="GEHiGU/wzMESSzNocXwPkaIr4XGdamS9vmVQvyC3AZJHmUXgJGyneI4jc1TC32WmhOi7y0hwZVPwY8duXyz3Tw==" saltValue="r4SSSOoEaaDH7zhAAgw2UA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="45">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="B108:B110"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="B92:B94"/>
+    <mergeCell ref="B95:B97"/>
+    <mergeCell ref="B98:B100"/>
+    <mergeCell ref="B101:B103"/>
+    <mergeCell ref="B111:B113"/>
+    <mergeCell ref="B114:B116"/>
+    <mergeCell ref="B117:B119"/>
+    <mergeCell ref="B120:B122"/>
+    <mergeCell ref="B125:B127"/>
     <mergeCell ref="B145:B147"/>
     <mergeCell ref="B148:B150"/>
     <mergeCell ref="B151:B153"/>
@@ -13638,42 +13683,6 @@
     <mergeCell ref="B134:B136"/>
     <mergeCell ref="B137:B139"/>
     <mergeCell ref="B142:B144"/>
-    <mergeCell ref="B111:B113"/>
-    <mergeCell ref="B114:B116"/>
-    <mergeCell ref="B117:B119"/>
-    <mergeCell ref="B120:B122"/>
-    <mergeCell ref="B125:B127"/>
-    <mergeCell ref="B108:B110"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="B92:B94"/>
-    <mergeCell ref="B95:B97"/>
-    <mergeCell ref="B98:B100"/>
-    <mergeCell ref="B101:B103"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -32805,8 +32814,8 @@
   </sheetPr>
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C11" activeCellId="2" sqref="C35 C23:F23 C11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -32917,16 +32926,16 @@
       <c r="B13" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="108" t="s">
         <v>77</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="108" t="s">
         <v>78</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="108" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="108" t="s">
         <v>80</v>
       </c>
       <c r="G13" s="11"/>
@@ -33124,7 +33133,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="6+Fd3+lM6F7CC5nfFjMDqczCxNwVKDBM6mVepSMFM7+v73SgdhSv8TfnfC8nlMe7xcq13q6MIjDLhTIelvMcKQ==" saltValue="kqEZBqN0TYQlZLQiK64T3Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="qnQzdOn5cQaLZSe3pL+La83oDabUmWeaBSVqPQgFolyKNa5SuNEdcmE0/iEmnqAIVofZiW6ppGiVvAzBGez/mA==" saltValue="FYKrJdzLs+Bg6aoEj0Uuxg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="69" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>

</xml_diff>